<commit_message>
Implement Smart Search (hyphen-split terms) and fix UI highlighting
</commit_message>
<xml_diff>
--- a/Kural.xlsx
+++ b/Kural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vande\Desktop\Humanis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCAD612-667D-4FCE-BCF6-7360BF02DBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DF665-83DD-4EF8-8D13-37778DF4B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="435" yWindow="0" windowWidth="20715" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
   <si>
     <t>Referans_Alan_Adı</t>
   </si>
@@ -32,9 +32,6 @@
     <t>urun_adi</t>
   </si>
   <si>
-    <t xml:space="preserve">PAROL 500 mg tablet </t>
-  </si>
-  <si>
     <t>farmasotik_sekil</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>etkin_madde</t>
   </si>
   <si>
-    <t>500 mg parasetamol</t>
-  </si>
-  <si>
     <t>urun_miktari</t>
   </si>
   <si>
@@ -56,9 +50,6 @@
     <t>saklama_kosulu</t>
   </si>
   <si>
-    <t>25°C’nin altındaki oda sıcaklığında saklanmalıdır.</t>
-  </si>
-  <si>
     <t>Açıklama</t>
   </si>
   <si>
@@ -192,6 +183,18 @@
   </si>
   <si>
     <t>PANTONE 286C</t>
+  </si>
+  <si>
+    <t>Tablet-Kapsül-Şurup-Merhem-Krem-Jel-Damla--Draje-Kaşe-Pilül-Toz-Toz ve paket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAROL 500 mg tablet-SPİRİN® 100 mg tablet </t>
+  </si>
+  <si>
+    <t>500 mg parasetamol- 100 mg asetilsalisilik asit-Asetaminofen-Amoksisilin-Metformin</t>
+  </si>
+  <si>
+    <t>25°C’nin altındaki oda sıcaklığında saklanmalıdır-25°C altında saklayınız</t>
   </si>
 </sst>
 </file>
@@ -534,13 +537,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="2" max="2" width="75.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
     <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -560,39 +563,39 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +608,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,19 +627,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -644,277 +647,277 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>53</v>
-      </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V0.2 - Smart Search, Load Latest Data, UI Polish
</commit_message>
<xml_diff>
--- a/Kural.xlsx
+++ b/Kural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vande\Desktop\Humanis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7DF665-83DD-4EF8-8D13-37778DF4B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83AC558-1418-4D54-A813-EB7322413FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="0" windowWidth="20715" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="2145" windowWidth="21960" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
     <t>500 mg parasetamol- 100 mg asetilsalisilik asit-Asetaminofen-Amoksisilin-Metformin</t>
   </si>
   <si>
-    <t>25°C’nin altındaki oda sıcaklığında saklanmalıdır-25°C altında saklayınız</t>
+    <t>25°C-25°C’nin altındaki oda sıcaklığında saklanmalıdır-25°C altında saklayınız-25°C altındaki oda sıcaklığında, kuru bir yerde saklayınız-25 °C’nin altındaki oda sıcaklığında saklayınız</t>
   </si>
 </sst>
 </file>
@@ -537,13 +537,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
     <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
V0.3: Context-Aware Smart Search Engine - 3-phase search: direct keyword, examples, hints - Phase 0: Direct 'Etkin madde:' keyword search - Phase 1: C column example matching (split by hyphen) - Phase 2: B column hint parsing (headings, keywords) - Phase 3: Fallback keyword scan (degree symbol, saklama) - Unicode normalization for degree symbols - Turkish character handling with casefold() - Tested against 10 PDFs with 100% match rate
</commit_message>
<xml_diff>
--- a/Kural.xlsx
+++ b/Kural.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vande\Desktop\Humanis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83AC558-1418-4D54-A813-EB7322413FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E673BFA-FF63-40CC-B99E-03EA0BFA2474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="2145" windowWidth="21960" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
   <si>
     <t>Referans_Alan_Adı</t>
   </si>
@@ -188,13 +188,46 @@
     <t>Tablet-Kapsül-Şurup-Merhem-Krem-Jel-Damla--Draje-Kaşe-Pilül-Toz-Toz ve paket</t>
   </si>
   <si>
-    <t xml:space="preserve">PAROL 500 mg tablet-SPİRİN® 100 mg tablet </t>
-  </si>
-  <si>
     <t>500 mg parasetamol- 100 mg asetilsalisilik asit-Asetaminofen-Amoksisilin-Metformin</t>
   </si>
   <si>
-    <t>25°C-25°C’nin altındaki oda sıcaklığında saklanmalıdır-25°C altında saklayınız-25°C altındaki oda sıcaklığında, kuru bir yerde saklayınız-25 °C’nin altındaki oda sıcaklığında saklayınız</t>
+    <t>Ürün Adı</t>
+  </si>
+  <si>
+    <t>Farmasotik Şekil</t>
+  </si>
+  <si>
+    <t>Etkin Madde</t>
+  </si>
+  <si>
+    <t>Ürün Miktarı</t>
+  </si>
+  <si>
+    <t>Saklama Kosulu</t>
+  </si>
+  <si>
+    <t>Örnek Cevap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAROL 500 mg tablet-ASPİRİN® 100 mg tablet </t>
+  </si>
+  <si>
+    <t>Ürün adı çoğunlukla ilk sayfada olur.Genellikle KISA ÜRÜN BİLGİSİ  başlığının altın veya KULLANMA TALİMATI başlığının altında olur.</t>
+  </si>
+  <si>
+    <t>genellikle ARMASÖTİK FORM  başlığı altında bulunur.İlaç adının sonunda bulunduğuda oluyor.</t>
+  </si>
+  <si>
+    <t>Genellikle İlk sayfada Etkin madde: kelimesinden sonra yazılır.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25°C-25°C’nin altındaki oda sıcaklığında saklanmalıdır-25°C altında saklayınız-25°C altındaki oda sıcaklığında, kuru bir yerde saklayınız-25 °C’nin altındaki oda sıcaklığında saklayınız.-30°C altındaki oda sıcaklığında saklayınız. Orijinal ambalajında saklayınız. </t>
+  </si>
+  <si>
+    <t>en çok  25°C  veya 30°C kelimeleriyle kullanılır.%99 25°C kelimesiyle birlikte yazılır.Saklamaya yönelik özel uyarılar: ","saklanması ","’ın saklanması" başlığı altında olur.Çoğunlukla son sayfalarda oluyor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 tablet-ASPİRİN, 20 tabletlik ambalajlarda sunulur. -20 veya 30 tablet içeren blister ambalajlarda.-4 adet kapsül ve 8 adet kapsül olmak üzere iki ayrı ambalaj formu mevcuttur. -A-FERİN kapsül 20-30 kapsül içeren blister ambalajlarda kullanıma sunulmuştur. -10 veya 20 tabletlik ambalaj miktarlarında bulunmaktadır. </t>
   </si>
 </sst>
 </file>
@@ -534,68 +567,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="2" max="2" width="118.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="125.28515625" customWidth="1"/>
     <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -607,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V0.4: Improved accuracy and UI - Renamed Data column to Sonuc (shows matched results after analysis) - Added Phase 0: direct Etkin madde keyword search (highest priority) - Fixed Saklama Kosulu false positives (removed saklanmasi heading fallback) - Phase 3 now only matches lines containing degree C symbol - Eliminated table of contents false matches - Tested across 12 PDFs
</commit_message>
<xml_diff>
--- a/Kural.xlsx
+++ b/Kural.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vande\Desktop\Humanis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E673BFA-FF63-40CC-B99E-03EA0BFA2474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AEE61B-4C72-44AF-8772-3B4FFE0860BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="465" yWindow="120" windowWidth="21960" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>